<commit_message>
Deploying to gh-pages from  @ 3819c61fbe18007217e1e406cac8c7089497d75d 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/9.3.1.xlsx
+++ b/en/downloads/data-excel/9.3.1.xlsx
@@ -167,7 +167,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -208,17 +208,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -527,9 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1173,14 +1178,14 @@
     <col min="16140" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="16"/>
@@ -1189,17 +1194,17 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9"/>
@@ -1213,7 +1218,7 @@
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -1227,8 +1232,9 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:13" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1268,8 +1274,11 @@
       <c r="M4" s="3">
         <v>2019</v>
       </c>
+      <c r="N4" s="3">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1307,10 +1316,13 @@
         <v>1.7</v>
       </c>
       <c r="M5" s="5">
-        <v>1.7</v>
+        <v>1.6</v>
+      </c>
+      <c r="N5" s="22">
+        <v>1.6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="12" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="6"/>
@@ -1324,7 +1336,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" ht="12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="12" x14ac:dyDescent="0.2">
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -1336,17 +1348,17 @@
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="1:13" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:13" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:13" ht="12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:14" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:14" ht="12" x14ac:dyDescent="0.2">
       <c r="G10" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="12" x14ac:dyDescent="0.2">
       <c r="G11" s="15"/>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L14" s="10" t="s">
         <v>8</v>
       </c>

</xml_diff>